<commit_message>
Algorithm bugged but excel output/input works
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Coding\Github_repo\Game-Planner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github_Repos\Game-Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D35ADFD-0B2C-48A0-9C90-2BC8BA297114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1096E54D-60C9-4AD9-B476-BBCC0C981666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C5BD4F56-FC55-4EC3-A309-E8CCA0F8A93A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C5BD4F56-FC55-4EC3-A309-E8CCA0F8A93A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>Team Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>A</t>
   </si>
@@ -61,6 +58,12 @@
     <t>H</t>
   </si>
   <si>
+    <t>Team List</t>
+  </si>
+  <si>
+    <t>Location List</t>
+  </si>
+  <si>
     <t>I</t>
   </si>
   <si>
@@ -68,42 +71,6 @@
   </si>
   <si>
     <t>K</t>
-  </si>
-  <si>
-    <t>Games:</t>
-  </si>
-  <si>
-    <t>A vs B</t>
-  </si>
-  <si>
-    <t>B vs C</t>
-  </si>
-  <si>
-    <t>C vs D</t>
-  </si>
-  <si>
-    <t>D vs E</t>
-  </si>
-  <si>
-    <t>E vs F</t>
-  </si>
-  <si>
-    <t>F vs G</t>
-  </si>
-  <si>
-    <t>G vs H</t>
-  </si>
-  <si>
-    <t>H vs I</t>
-  </si>
-  <si>
-    <t>I vs J</t>
-  </si>
-  <si>
-    <t>J vs K</t>
-  </si>
-  <si>
-    <t>K vs A</t>
   </si>
 </sst>
 </file>
@@ -142,7 +109,7 @@
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,108 +428,87 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
outputs to excel sheet properly Still bugged
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github_Repos\Game-Planner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Coding\Github_repo\Game-Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1096E54D-60C9-4AD9-B476-BBCC0C981666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A26075-F652-48F1-9240-72E31BAAB033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C5BD4F56-FC55-4EC3-A309-E8CCA0F8A93A}"/>
+    <workbookView xWindow="0" yWindow="1848" windowWidth="12960" windowHeight="8964" xr2:uid="{C5BD4F56-FC55-4EC3-A309-E8CCA0F8A93A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>A</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>four</t>
   </si>
 </sst>
 </file>
@@ -428,15 +440,15 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -444,69 +456,69 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Combined the graphical interface with the algorithm
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Coding\Github_repo\Game-Planner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Coding\Github_repo\Game-Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D35ADFD-0B2C-48A0-9C90-2BC8BA297114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEF751F-8C3F-4101-877F-7D851232029C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C5BD4F56-FC55-4EC3-A309-E8CCA0F8A93A}"/>
+    <workbookView xWindow="0" yWindow="1848" windowWidth="12960" windowHeight="8964" xr2:uid="{C5BD4F56-FC55-4EC3-A309-E8CCA0F8A93A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Team Name</t>
   </si>
@@ -70,40 +70,19 @@
     <t>K</t>
   </si>
   <si>
-    <t>Games:</t>
-  </si>
-  <si>
-    <t>A vs B</t>
-  </si>
-  <si>
-    <t>B vs C</t>
-  </si>
-  <si>
-    <t>C vs D</t>
-  </si>
-  <si>
-    <t>D vs E</t>
-  </si>
-  <si>
-    <t>E vs F</t>
-  </si>
-  <si>
-    <t>F vs G</t>
-  </si>
-  <si>
-    <t>G vs H</t>
-  </si>
-  <si>
-    <t>H vs I</t>
-  </si>
-  <si>
-    <t>I vs J</t>
-  </si>
-  <si>
-    <t>J vs K</t>
-  </si>
-  <si>
-    <t>K vs A</t>
+    <t>Locations</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L4</t>
   </si>
 </sst>
 </file>
@@ -461,7 +440,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,56 +492,35 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added additional outputs Improve GUI (still ugly)
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Coding\Github_repo\Game-Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC66E1A9-CD88-49CF-B5B5-C45236578B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C225375A-94F6-4932-A04B-6C1E47F06F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="12960" windowHeight="8964" xr2:uid="{C5BD4F56-FC55-4EC3-A309-E8CCA0F8A93A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C5BD4F56-FC55-4EC3-A309-E8CCA0F8A93A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Team Name</t>
   </si>
@@ -40,49 +40,70 @@
     <t>Locations</t>
   </si>
   <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>L4</t>
-  </si>
-  <si>
-    <t>Team One</t>
-  </si>
-  <si>
-    <t>Team Two</t>
-  </si>
-  <si>
-    <t>Team Three</t>
-  </si>
-  <si>
-    <t>Team Four</t>
-  </si>
-  <si>
-    <t>Team Five</t>
-  </si>
-  <si>
-    <t>Team Six</t>
-  </si>
-  <si>
-    <t>Team Seven</t>
-  </si>
-  <si>
-    <t>Team Eight</t>
-  </si>
-  <si>
-    <t>Team Nin</t>
-  </si>
-  <si>
-    <t>Team Ten</t>
-  </si>
-  <si>
-    <t>Team Eleven</t>
+    <t>Deziree Niki</t>
+  </si>
+  <si>
+    <t>Sue Madelon</t>
+  </si>
+  <si>
+    <t>Ridge Allissa</t>
+  </si>
+  <si>
+    <t>Thad Soan</t>
+  </si>
+  <si>
+    <t>Claudine</t>
+  </si>
+  <si>
+    <t>Skylar</t>
+  </si>
+  <si>
+    <t>Edmé</t>
+  </si>
+  <si>
+    <t>Irvin</t>
+  </si>
+  <si>
+    <t>Flavien</t>
+  </si>
+  <si>
+    <t>Miranda</t>
+  </si>
+  <si>
+    <t>Placide</t>
+  </si>
+  <si>
+    <t>Dory</t>
+  </si>
+  <si>
+    <t>Stefani</t>
+  </si>
+  <si>
+    <t>Becky</t>
+  </si>
+  <si>
+    <t>Roswell</t>
+  </si>
+  <si>
+    <t>Skye Annabelle</t>
+  </si>
+  <si>
+    <t>Craig</t>
+  </si>
+  <si>
+    <t>Carrol</t>
+  </si>
+  <si>
+    <t>Ultman Park</t>
+  </si>
+  <si>
+    <t>Merry Mark</t>
+  </si>
+  <si>
+    <t>Ken Ross Park</t>
+  </si>
+  <si>
+    <t>Mulligan Park</t>
   </si>
 </sst>
 </file>
@@ -437,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F5255F-776E-4042-BB3A-94D70B4B652E}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,69 +479,104 @@
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>